<commit_message>
Final Upload for Project Submission
</commit_message>
<xml_diff>
--- a/StatePopulation.xlsx
+++ b/StatePopulation.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dane\Desktop\WriteToDatabase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FAEC1EA1-322E-48A1-BBA1-56DF64DE44FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95650942-ABD1-4A53-B89F-C628483D7F6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="StatePopulation" sheetId="1" r:id="rId1"/>
@@ -211,7 +211,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="167" formatCode="0.0"/>
+  </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -689,8 +692,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1045,12 +1049,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:E58"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="14.6328125" customWidth="1"/>
+    <col min="3" max="3" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9.54296875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -1073,16 +1084,16 @@
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>331501080</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>331893745</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <v>853448</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="1">
         <v>3433943</v>
       </c>
     </row>
@@ -1090,16 +1101,16 @@
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>57525633</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <v>57159838</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="1">
         <v>148129</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="1">
         <v>601644</v>
       </c>
     </row>
@@ -1107,16 +1118,16 @@
       <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>68935174</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <v>68841444</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="1">
         <v>193237</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="1">
         <v>761784</v>
       </c>
     </row>
@@ -1124,16 +1135,16 @@
       <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>126409007</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1">
         <v>127225329</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="1">
         <v>337628</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="1">
         <v>1366769</v>
       </c>
     </row>
@@ -1141,16 +1152,16 @@
       <c r="A6" t="s">
         <v>9</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
         <v>78631266</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="1">
         <v>78667134</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="1">
         <v>174454</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="1">
         <v>703746</v>
       </c>
     </row>
@@ -1158,16 +1169,16 @@
       <c r="A7" t="s">
         <v>10</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="1">
         <v>5024803</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="1">
         <v>5039877</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="1">
         <v>16148</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="1">
         <v>64868</v>
       </c>
     </row>
@@ -1175,16 +1186,16 @@
       <c r="A8" t="s">
         <v>11</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="1">
         <v>732441</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="1">
         <v>732673</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="1">
         <v>1384</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="1">
         <v>5641</v>
       </c>
     </row>
@@ -1192,16 +1203,16 @@
       <c r="A9" t="s">
         <v>12</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="1">
         <v>7177986</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="1">
         <v>7276316</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="1">
         <v>18340</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="1">
         <v>75665</v>
       </c>
     </row>
@@ -1209,16 +1220,16 @@
       <c r="A10" t="s">
         <v>13</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="1">
         <v>3012232</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="1">
         <v>3025891</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="1">
         <v>9449</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="1">
         <v>38257</v>
       </c>
     </row>
@@ -1226,16 +1237,16 @@
       <c r="A11" t="s">
         <v>14</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="1">
         <v>39499738</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="1">
         <v>39237836</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="1">
         <v>81738</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="1">
         <v>332337</v>
       </c>
     </row>
@@ -1243,16 +1254,16 @@
       <c r="A12" t="s">
         <v>15</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="1">
         <v>5784308</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="1">
         <v>5812069</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="1">
         <v>11835</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="1">
         <v>47988</v>
       </c>
     </row>
@@ -1260,16 +1271,16 @@
       <c r="A13" t="s">
         <v>16</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="1">
         <v>3600260</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="1">
         <v>3605597</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="1">
         <v>9428</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="1">
         <v>37646</v>
       </c>
     </row>
@@ -1277,16 +1288,16 @@
       <c r="A14" t="s">
         <v>17</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="1">
         <v>991886</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="1">
         <v>1003384</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="1">
         <v>2649</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="1">
         <v>11655</v>
       </c>
     </row>
@@ -1294,16 +1305,16 @@
       <c r="A15" t="s">
         <v>18</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="1">
         <v>690093</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="1">
         <v>670050</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="1">
         <v>1387</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="1">
         <v>6552</v>
       </c>
     </row>
@@ -1311,16 +1322,16 @@
       <c r="A16" t="s">
         <v>19</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="1">
         <v>21569932</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="1">
         <v>21781128</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="1">
         <v>63596</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="1">
         <v>255553</v>
       </c>
     </row>
@@ -1328,16 +1339,16 @@
       <c r="A17" t="s">
         <v>20</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="1">
         <v>10725800</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="1">
         <v>10799566</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="1">
         <v>25664</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="1">
         <v>105276</v>
       </c>
     </row>
@@ -1345,16 +1356,16 @@
       <c r="A18" t="s">
         <v>21</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="1">
         <v>1451911</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="1">
         <v>1441553</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="1">
         <v>3773</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="1">
         <v>14648</v>
       </c>
     </row>
@@ -1362,16 +1373,16 @@
       <c r="A19" t="s">
         <v>22</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="1">
         <v>1847772</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="1">
         <v>1900923</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="1">
         <v>4450</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="1">
         <v>16918</v>
       </c>
     </row>
@@ -1379,16 +1390,16 @@
       <c r="A20" t="s">
         <v>23</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="1">
         <v>12785245</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="1">
         <v>12671469</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="1">
         <v>32486</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="1">
         <v>130319</v>
       </c>
     </row>
@@ -1396,16 +1407,16 @@
       <c r="A21" t="s">
         <v>24</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="1">
         <v>6785644</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="1">
         <v>6805985</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="1">
         <v>19664</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="1">
         <v>76906</v>
       </c>
     </row>
@@ -1413,16 +1424,16 @@
       <c r="A22" t="s">
         <v>25</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="1">
         <v>3188669</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="1">
         <v>3193079</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="1">
         <v>9005</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="1">
         <v>35538</v>
       </c>
     </row>
@@ -1430,16 +1441,16 @@
       <c r="A23" t="s">
         <v>26</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="1">
         <v>2935880</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="1">
         <v>2934582</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="1">
         <v>7981</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="1">
         <v>31407</v>
       </c>
     </row>
@@ -1447,16 +1458,16 @@
       <c r="A24" t="s">
         <v>27</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="1">
         <v>4503958</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="1">
         <v>4509394</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="1">
         <v>14557</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="1">
         <v>56853</v>
       </c>
     </row>
@@ -1464,16 +1475,16 @@
       <c r="A25" t="s">
         <v>28</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="1">
         <v>4651203</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="1">
         <v>4624047</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="1">
         <v>13460</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="1">
         <v>55335</v>
       </c>
     </row>
@@ -1481,16 +1492,16 @@
       <c r="A26" t="s">
         <v>29</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="1">
         <v>1362280</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="1">
         <v>1372247</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="1">
         <v>4507</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="1">
         <v>17635</v>
       </c>
     </row>
@@ -1498,16 +1509,16 @@
       <c r="A27" t="s">
         <v>30</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="1">
         <v>6172679</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="1">
         <v>6165129</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="1">
         <v>15128</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="1">
         <v>61654</v>
       </c>
     </row>
@@ -1515,16 +1526,16 @@
       <c r="A28" t="s">
         <v>31</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="1">
         <v>7022220</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="1">
         <v>6984723</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="1">
         <v>17353</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="1">
         <v>70431</v>
       </c>
     </row>
@@ -1532,16 +1543,16 @@
       <c r="A29" t="s">
         <v>32</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="1">
         <v>10067664</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="1">
         <v>10050811</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="1">
         <v>29450</v>
       </c>
-      <c r="E29">
+      <c r="E29" s="1">
         <v>117336</v>
       </c>
     </row>
@@ -1549,16 +1560,16 @@
       <c r="A30" t="s">
         <v>33</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="1">
         <v>5707165</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="1">
         <v>5707390</v>
       </c>
-      <c r="D30">
+      <c r="D30" s="1">
         <v>13403</v>
       </c>
-      <c r="E30">
+      <c r="E30" s="1">
         <v>53578</v>
       </c>
     </row>
@@ -1566,16 +1577,16 @@
       <c r="A31" t="s">
         <v>34</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="1">
         <v>2956870</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="1">
         <v>2949965</v>
       </c>
-      <c r="D31">
+      <c r="D31" s="1">
         <v>9793</v>
       </c>
-      <c r="E31">
+      <c r="E31" s="1">
         <v>38194</v>
       </c>
     </row>
@@ -1583,16 +1594,16 @@
       <c r="A32" t="s">
         <v>35</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="1">
         <v>6154481</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="1">
         <v>6168187</v>
       </c>
-      <c r="D32">
+      <c r="D32" s="1">
         <v>18574</v>
       </c>
-      <c r="E32">
+      <c r="E32" s="1">
         <v>73333</v>
       </c>
     </row>
@@ -1600,16 +1611,16 @@
       <c r="A33" t="s">
         <v>36</v>
       </c>
-      <c r="B33">
+      <c r="B33" s="1">
         <v>1086193</v>
       </c>
-      <c r="C33">
+      <c r="C33" s="1">
         <v>1104271</v>
       </c>
-      <c r="D33">
+      <c r="D33" s="1">
         <v>3050</v>
       </c>
-      <c r="E33">
+      <c r="E33" s="1">
         <v>12022</v>
       </c>
     </row>
@@ -1617,16 +1628,16 @@
       <c r="A34" t="s">
         <v>37</v>
       </c>
-      <c r="B34">
+      <c r="B34" s="1">
         <v>1961455</v>
       </c>
-      <c r="C34">
+      <c r="C34" s="1">
         <v>1963692</v>
       </c>
-      <c r="D34">
+      <c r="D34" s="1">
         <v>5041</v>
       </c>
-      <c r="E34">
+      <c r="E34" s="1">
         <v>19213</v>
       </c>
     </row>
@@ -1634,16 +1645,16 @@
       <c r="A35" t="s">
         <v>38</v>
       </c>
-      <c r="B35">
+      <c r="B35" s="1">
         <v>3114071</v>
       </c>
-      <c r="C35">
+      <c r="C35" s="1">
         <v>3143991</v>
       </c>
-      <c r="D35">
+      <c r="D35" s="1">
         <v>7894</v>
       </c>
-      <c r="E35">
+      <c r="E35" s="1">
         <v>31808</v>
       </c>
     </row>
@@ -1651,16 +1662,16 @@
       <c r="A36" t="s">
         <v>39</v>
       </c>
-      <c r="B36">
+      <c r="B36" s="1">
         <v>1377848</v>
       </c>
-      <c r="C36">
+      <c r="C36" s="1">
         <v>1388992</v>
       </c>
-      <c r="D36">
+      <c r="D36" s="1">
         <v>3659</v>
       </c>
-      <c r="E36">
+      <c r="E36" s="1">
         <v>15158</v>
       </c>
     </row>
@@ -1668,16 +1679,16 @@
       <c r="A37" t="s">
         <v>40</v>
       </c>
-      <c r="B37">
+      <c r="B37" s="1">
         <v>9279743</v>
       </c>
-      <c r="C37">
+      <c r="C37" s="1">
         <v>9267130</v>
       </c>
-      <c r="D37">
+      <c r="D37" s="1">
         <v>22016</v>
       </c>
-      <c r="E37">
+      <c r="E37" s="1">
         <v>90557</v>
       </c>
     </row>
@@ -1685,16 +1696,16 @@
       <c r="A38" t="s">
         <v>41</v>
       </c>
-      <c r="B38">
+      <c r="B38" s="1">
         <v>2117566</v>
       </c>
-      <c r="C38">
+      <c r="C38" s="1">
         <v>2115877</v>
       </c>
-      <c r="D38">
+      <c r="D38" s="1">
         <v>5808</v>
       </c>
-      <c r="E38">
+      <c r="E38" s="1">
         <v>23082</v>
       </c>
     </row>
@@ -1702,16 +1713,16 @@
       <c r="A39" t="s">
         <v>42</v>
       </c>
-      <c r="B39">
+      <c r="B39" s="1">
         <v>20154933</v>
       </c>
-      <c r="C39">
+      <c r="C39" s="1">
         <v>19835913</v>
       </c>
-      <c r="D39">
+      <c r="D39" s="1">
         <v>46447</v>
       </c>
-      <c r="E39">
+      <c r="E39" s="1">
         <v>192137</v>
       </c>
     </row>
@@ -1719,16 +1730,16 @@
       <c r="A40" t="s">
         <v>43</v>
       </c>
-      <c r="B40">
+      <c r="B40" s="1">
         <v>10457177</v>
       </c>
-      <c r="C40">
+      <c r="C40" s="1">
         <v>10551162</v>
       </c>
-      <c r="D40">
+      <c r="D40" s="1">
         <v>28852</v>
       </c>
-      <c r="E40">
+      <c r="E40" s="1">
         <v>115709</v>
       </c>
     </row>
@@ -1736,16 +1747,16 @@
       <c r="A41" t="s">
         <v>44</v>
       </c>
-      <c r="B41">
+      <c r="B41" s="1">
         <v>778962</v>
       </c>
-      <c r="C41">
+      <c r="C41" s="1">
         <v>774948</v>
       </c>
-      <c r="D41">
+      <c r="D41" s="1">
         <v>2116</v>
       </c>
-      <c r="E41">
+      <c r="E41" s="1">
         <v>7588</v>
       </c>
     </row>
@@ -1753,16 +1764,16 @@
       <c r="A42" t="s">
         <v>45</v>
       </c>
-      <c r="B42">
+      <c r="B42" s="1">
         <v>11790587</v>
       </c>
-      <c r="C42">
+      <c r="C42" s="1">
         <v>11780017</v>
       </c>
-      <c r="D42">
+      <c r="D42" s="1">
         <v>36827</v>
       </c>
-      <c r="E42">
+      <c r="E42" s="1">
         <v>144406</v>
       </c>
     </row>
@@ -1770,16 +1781,16 @@
       <c r="A43" t="s">
         <v>46</v>
       </c>
-      <c r="B43">
+      <c r="B43" s="1">
         <v>3962031</v>
       </c>
-      <c r="C43">
+      <c r="C43" s="1">
         <v>3986639</v>
       </c>
-      <c r="D43">
+      <c r="D43" s="1">
         <v>11925</v>
       </c>
-      <c r="E43">
+      <c r="E43" s="1">
         <v>48995</v>
       </c>
     </row>
@@ -1787,16 +1798,16 @@
       <c r="A44" t="s">
         <v>47</v>
       </c>
-      <c r="B44">
+      <c r="B44" s="1">
         <v>4241544</v>
       </c>
-      <c r="C44">
+      <c r="C44" s="1">
         <v>4246155</v>
       </c>
-      <c r="D44">
+      <c r="D44" s="1">
         <v>11334</v>
       </c>
-      <c r="E44">
+      <c r="E44" s="1">
         <v>44592</v>
       </c>
     </row>
@@ -1804,16 +1815,16 @@
       <c r="A45" t="s">
         <v>48</v>
       </c>
-      <c r="B45">
+      <c r="B45" s="1">
         <v>12989625</v>
       </c>
-      <c r="C45">
+      <c r="C45" s="1">
         <v>12964056</v>
       </c>
-      <c r="D45">
+      <c r="D45" s="1">
         <v>39879</v>
       </c>
-      <c r="E45">
+      <c r="E45" s="1">
         <v>159229</v>
       </c>
     </row>
@@ -1821,16 +1832,16 @@
       <c r="A46" t="s">
         <v>49</v>
       </c>
-      <c r="B46">
+      <c r="B46" s="1">
         <v>1096229</v>
       </c>
-      <c r="C46">
+      <c r="C46" s="1">
         <v>1095610</v>
       </c>
-      <c r="D46">
+      <c r="D46" s="1">
         <v>3036</v>
       </c>
-      <c r="E46">
+      <c r="E46" s="1">
         <v>11967</v>
       </c>
     </row>
@@ -1838,16 +1849,16 @@
       <c r="A47" t="s">
         <v>50</v>
       </c>
-      <c r="B47">
+      <c r="B47" s="1">
         <v>5130729</v>
       </c>
-      <c r="C47">
+      <c r="C47" s="1">
         <v>5190705</v>
       </c>
-      <c r="D47">
+      <c r="D47" s="1">
         <v>15134</v>
       </c>
-      <c r="E47">
+      <c r="E47" s="1">
         <v>62520</v>
       </c>
     </row>
@@ -1855,16 +1866,16 @@
       <c r="A48" t="s">
         <v>51</v>
       </c>
-      <c r="B48">
+      <c r="B48" s="1">
         <v>887099</v>
       </c>
-      <c r="C48">
+      <c r="C48" s="1">
         <v>895376</v>
       </c>
-      <c r="D48">
+      <c r="D48" s="1">
         <v>2496</v>
       </c>
-      <c r="E48">
+      <c r="E48" s="1">
         <v>9175</v>
       </c>
     </row>
@@ -1872,16 +1883,16 @@
       <c r="A49" t="s">
         <v>52</v>
       </c>
-      <c r="B49">
+      <c r="B49" s="1">
         <v>6920119</v>
       </c>
-      <c r="C49">
+      <c r="C49" s="1">
         <v>6975218</v>
       </c>
-      <c r="D49">
+      <c r="D49" s="1">
         <v>21873</v>
       </c>
-      <c r="E49">
+      <c r="E49" s="1">
         <v>84944</v>
       </c>
     </row>
@@ -1889,16 +1900,16 @@
       <c r="A50" t="s">
         <v>53</v>
       </c>
-      <c r="B50">
+      <c r="B50" s="1">
         <v>29217653</v>
       </c>
-      <c r="C50">
+      <c r="C50" s="1">
         <v>29527941</v>
       </c>
-      <c r="D50">
+      <c r="D50" s="1">
         <v>60137</v>
       </c>
-      <c r="E50">
+      <c r="E50" s="1">
         <v>248605</v>
       </c>
     </row>
@@ -1906,16 +1917,16 @@
       <c r="A51" t="s">
         <v>54</v>
       </c>
-      <c r="B51">
+      <c r="B51" s="1">
         <v>3281684</v>
       </c>
-      <c r="C51">
+      <c r="C51" s="1">
         <v>3337975</v>
       </c>
-      <c r="D51">
+      <c r="D51" s="1">
         <v>5705</v>
       </c>
-      <c r="E51">
+      <c r="E51" s="1">
         <v>22167</v>
       </c>
     </row>
@@ -1923,16 +1934,16 @@
       <c r="A52" t="s">
         <v>55</v>
       </c>
-      <c r="B52">
+      <c r="B52" s="1">
         <v>642495</v>
       </c>
-      <c r="C52">
+      <c r="C52" s="1">
         <v>645570</v>
       </c>
-      <c r="D52">
+      <c r="D52" s="1">
         <v>1804</v>
       </c>
-      <c r="E52">
+      <c r="E52" s="1">
         <v>6884</v>
       </c>
     </row>
@@ -1940,16 +1951,16 @@
       <c r="A53" t="s">
         <v>56</v>
       </c>
-      <c r="B53">
+      <c r="B53" s="1">
         <v>8632044</v>
       </c>
-      <c r="C53">
+      <c r="C53" s="1">
         <v>8642274</v>
       </c>
-      <c r="D53">
+      <c r="D53" s="1">
         <v>20881</v>
       </c>
-      <c r="E53">
+      <c r="E53" s="1">
         <v>84697</v>
       </c>
     </row>
@@ -1957,16 +1968,16 @@
       <c r="A54" t="s">
         <v>57</v>
       </c>
-      <c r="B54">
+      <c r="B54" s="1">
         <v>7718785</v>
       </c>
-      <c r="C54">
+      <c r="C54" s="1">
         <v>7738692</v>
       </c>
-      <c r="D54">
+      <c r="D54" s="1">
         <v>17643</v>
       </c>
-      <c r="E54">
+      <c r="E54" s="1">
         <v>70836</v>
       </c>
     </row>
@@ -1974,16 +1985,16 @@
       <c r="A55" t="s">
         <v>58</v>
       </c>
-      <c r="B55">
+      <c r="B55" s="1">
         <v>1789798</v>
       </c>
-      <c r="C55">
+      <c r="C55" s="1">
         <v>1782959</v>
       </c>
-      <c r="D55">
+      <c r="D55" s="1">
         <v>6995</v>
       </c>
-      <c r="E55">
+      <c r="E55" s="1">
         <v>27102</v>
       </c>
     </row>
@@ -1991,16 +2002,16 @@
       <c r="A56" t="s">
         <v>59</v>
       </c>
-      <c r="B56">
+      <c r="B56" s="1">
         <v>5892323</v>
       </c>
-      <c r="C56">
+      <c r="C56" s="1">
         <v>5895908</v>
       </c>
-      <c r="D56">
+      <c r="D56" s="1">
         <v>16194</v>
       </c>
-      <c r="E56">
+      <c r="E56" s="1">
         <v>62985</v>
       </c>
     </row>
@@ -2008,16 +2019,16 @@
       <c r="A57" t="s">
         <v>60</v>
       </c>
-      <c r="B57">
+      <c r="B57" s="1">
         <v>577267</v>
       </c>
-      <c r="C57">
+      <c r="C57" s="1">
         <v>578803</v>
       </c>
-      <c r="D57">
+      <c r="D57" s="1">
         <v>1500</v>
       </c>
-      <c r="E57">
+      <c r="E57" s="1">
         <v>6042</v>
       </c>
     </row>
@@ -2025,16 +2036,16 @@
       <c r="A58" t="s">
         <v>61</v>
       </c>
-      <c r="B58">
+      <c r="B58" s="1">
         <v>3281538</v>
       </c>
-      <c r="C58">
+      <c r="C58" s="1">
         <v>3263584</v>
       </c>
-      <c r="D58">
+      <c r="D58" s="1">
         <v>7324</v>
       </c>
-      <c r="E58">
+      <c r="E58" s="1">
         <v>32710</v>
       </c>
     </row>

</xml_diff>